<commit_message>
updated logo and placeholder
</commit_message>
<xml_diff>
--- a/static/assets/uploads/PCOS_Template.xlsx
+++ b/static/assets/uploads/PCOS_Template.xlsx
@@ -1,42 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisJ\Desktop\PCOS-Diagnose-SVM-DT\PCOS-Diagnosing-SVM-DT\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colasino\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB271F24-4566-4B52-B8C0-C8BAA1F1ED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852CCE1-D7B4-48AA-9DF8-E3E598E7DB8A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Patient File No.</t>
   </si>
@@ -204,11 +192,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +215,11 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -252,8 +245,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -274,8 +268,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,60 +581,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A46F1CA-6E2D-45D9-A3CD-231C4EE18203}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AX5" sqref="AX5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" style="3" customWidth="1"/>
     <col min="16" max="16" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="9.140625" style="3"/>
+    <col min="42" max="42" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.33203125" style="3" customWidth="1"/>
+    <col min="44" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>51</v>
       </c>
@@ -898,6 +894,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A7:AP7">
+    <sortCondition ref="A6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Table change in api.py
</commit_message>
<xml_diff>
--- a/static/assets/uploads/PCOS_Template.xlsx
+++ b/static/assets/uploads/PCOS_Template.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colasino\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisJ\Desktop\PCOS-Diagnose-SVM-DT\PCOS-Diagnosing-SVM-DT\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB271F24-4566-4B52-B8C0-C8BAA1F1ED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6852CCE1-D7B4-48AA-9DF8-E3E598E7DB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Patient File No.</t>
   </si>
@@ -192,11 +204,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,11 +227,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -245,9 +252,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -268,9 +274,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -581,61 +586,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A46F1CA-6E2D-45D9-A3CD-231C4EE18203}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AX5" sqref="AX5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="3" customWidth="1"/>
     <col min="16" max="16" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.33203125" style="3" customWidth="1"/>
-    <col min="44" max="16384" width="9.109375" style="3"/>
+    <col min="42" max="42" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +767,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>51</v>
       </c>
@@ -894,9 +898,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A7:AP7">
-    <sortCondition ref="A6"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>